<commit_message>
New place of entry inferences
</commit_message>
<xml_diff>
--- a/inferences/jesuita-entrada-Coimbra-extra_info.xlsx
+++ b/inferences/jesuita-entrada-Coimbra-extra_info.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="jesuita_entrada_Coimbra_extra" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="jesuita_entrada_Coimbra_extra" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,683 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>jesuita-entrada.obs</t>
+          <t>jesuita-entrada.original</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>jesuita-entrada.original.comment</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>jesuita-entrada.extra_info</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>deh-lourenco-mexia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Lourenço Mexia</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>15600314</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Domingues &amp; O Neil, IV: 2645. MMHM:p.226</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>{'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date', 'comment': 'ou 15600325 ou Coimbra, 25-03-1560 MMHM'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Domingues &amp; O Neil, IV: 2645. MMHM:p.226', 'original': '?'}, 'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>deh-francisco-vieira</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Francisco Vieira</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>15740200</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Está no "Catálogo delos Padres y Hermanos dela Provincia de Portugal a 12 de Enero de 1579",Lus. 39 p.3v, nos estudantes de Filosofia do segundo curso</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': 'Está no "Catálogo delos Padres y Hermanos dela Provincia de Portugal a 12 de Enero de 1579",Lus. 39 p.3v, nos estudantes de Filosofia do segundo curso', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>deh-manuel-gaspar</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Manuel Gaspar</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>15750926</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Schutte, Monumenta historica japoniae I.,p.1180</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Schutte, Monumenta historica japoniae I.,p.1180', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>deh-antonio-de-almeida</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>António de Almeida</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15760104</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>"Catálogo delos Padres y Hermanos dela Provincia de Portugal a 12 de Enero de 1579" Lus. 39, 3v, estudante de filosofia, 1ºcurso</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '"Catálogo delos Padres y Hermanos dela Provincia de Portugal a 12 de Enero de 1579" Lus. 39, 3v, estudante de filosofia, 1ºcurso', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>deh-joao-da-rocha</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>João da Rocha</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1583</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Em Coimbra no ano de 1582 segundo a Carta Annua de 1623 BA</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>{'obs': {'kleio_element_name': 'obs', 'kleio_element_class': 'obs', 'entity_attr_name': 'obs', 'entity_column_class': 'obs'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Em Coimbra no ano de 1582 segundo a Carta Annua de 1623 BA', 'original': '?'}, 'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>deh-mateus-de-couros</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mateus de Couros</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>15831222</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 MMHM:p.94 (ARSI Japsin 35 13)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>{'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 MMHM:p.94 (ARSI Japsin 35 13)', 'original': '?'}, 'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>deh-andre-palmeiro</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>André Palmeiro</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>15840114</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Segundo Dominguez &amp; O Neil, V.III,p.2961. Franco Imagem...Coimbra,II,4,c.36,p.575</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Segundo Dominguez &amp; O Neil, V.III,p.2961. Franco Imagem...Coimbra,II,4,c.36,p.575', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>deh-sebastiao-vieira</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sebastião Vieira</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>15910203</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>([Schütte, 1975, p. 1321] Sebastião Vieira, nasc Castro de Aire, Lamego, E. Coimbra 3-2-1591</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '([Schütte, 1975, p. 1321] Sebastião Vieira, nasc Castro de Aire, Lamego, E. Coimbra 3-2-1591', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>deh-manuel-dias-o-novo</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Manuel Dias, o Novo</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>15930202</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Segungo Dominguez, J. M., &amp; O’Neill, C. (2001) II, 1113</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Segungo Dominguez, J. M., &amp; O’Neill, C. (2001) II, 1113', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>deh-simao-da-cunha</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Simão da Cunha</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>16060113</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Dehergne não especifica local, Brockey estudos Filosofia e Teologia em Coimbra</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>{'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Dehergne não especifica local, Brockey estudos Filosofia e Teologia em Coimbra', 'original': '?'}, 'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>deh-antonio-de-gouvea</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>António de Gouveia</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>16080502</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 (Franco, 1719, t.II, p. 612)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date', 'comment': 'ou 16090502 reentrou em 1611 não se sabe onde'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 (Franco, 1719, t.II, p. 612)', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>deh-gaspar-do-amaral</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Gaspar do Amaral</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>16080601</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>[Adicionado a partir de Franco, Imagem...Coimbra, II, 522] @wikidata:Q45412</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date', 'comment': 'MMHM:p.8'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '[Adicionado a partir de Franco, Imagem...Coimbra, II, 522] @wikidata:Q45412', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>deh-francisco-furtado</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Francisco Furtado</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1610</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 """Franco, Imagem...Coimbra, v.2 p.616; Barbosa Machado, v.3"""</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 """Franco, Imagem...Coimbra, v.2 p.616; Barbosa Machado, v.3"""', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>deh-sebastiao-da-maia</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sebastião da Maia</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>16110000</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 MMHM:p.205 (Sebastian da Maia, da Maya, d'Amaya)</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': "@wikidata:Q45412 MMHM:p.205 (Sebastian da Maia, da Maya, d'Amaya)", 'original': '?'}, 'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>deh-gabriel-de-magalhaes</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Gabriel de Magalhães</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>16250000</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Segundo Louis Buglio 1688</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>{'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Segundo Louis Buglio 1688', 'original': '?'}, 'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>deh-matias-da-maia</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Matias da Maia</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>16290510</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 MMHM:p.203 (Matias d'Amaia), Schutte, Monumenta historica japoniae I.1234</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>{'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': "@wikidata:Q45412 MMHM:p.203 (Matias d'Amaia), Schutte, Monumenta historica japoniae I.1234", 'original': '?'}, 'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>deh-adriano-pestana</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Adriano Pestana</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>16350000</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Ver Brockey, p.230 cit. Carta de A.P. a Viteleschi, de Coimbra, 26 Agosto 1640</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Ver Brockey, p.230 cit. Carta de A.P. a Viteleschi, de Coimbra, 26 Agosto 1640', 'original': '?'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>deh-andre-ferrao</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>André Ferrão</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1640</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>@wikidata:Q45412 Brockey, cap.6 n.95</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>{'class': {'kleio_element_name': 'class', 'kleio_element_class': 'class', 'entity_attr_name': 'class', 'entity_column_class': 'class'}, 'id': {'kleio_element_name': 'id', 'kleio_element_class': 'id', 'entity_attr_name': 'id', 'entity_column_class': 'id'}, 'the_date': {'kleio_element_name': 'date', 'kleio_element_class': 'date', 'entity_attr_name': 'date', 'entity_column_class': 'date'}, 'the_type': {'kleio_element_name': 'tipo', 'kleio_element_class': 'type', 'entity_attr_name': 'type', 'entity_column_class': 'type'}, 'obs': {'kleio_element_name': 'obs', 'kleio_element_class': 'obs', 'entity_attr_name': 'obs', 'entity_column_class': 'obs'}, 'entity': {'kleio_element_name': 'entity', 'kleio_element_class': 'entity', 'entity_attr_name': 'entity', 'entity_column_class': 'entity'}, 'the_value': {'kleio_element_name': 'valor', 'kleio_element_class': 'value', 'entity_attr_name': 'value', 'entity_column_class': 'value', 'comment': '@wikidata:Q45412 Brockey, cap.6 n.95', 'original': '?'}}</t>
         </is>
       </c>
     </row>

</xml_diff>